<commit_message>
fig supp mat percentage of ones
</commit_message>
<xml_diff>
--- a/rawdata/supplementary_material_V3.xlsx
+++ b/rawdata/supplementary_material_V3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3D8AD2-090D-45B3-AACD-11B1DE0AB0BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478406D1-2B7C-4753-9BC6-23FD845C1050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="765" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="765" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring system" sheetId="1" r:id="rId1"/>
@@ -65,40 +65,6 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Auteur</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5042FC93-8E76-4022-B536-2511A0624CBD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Auteur:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-NOTE THE REVIEWED VERSION</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
@@ -327,7 +293,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
@@ -748,7 +714,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
@@ -783,7 +749,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Auteur</author>
@@ -5645,6 +5611,12 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5654,11 +5626,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5666,22 +5638,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5691,6 +5651,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6143,10 +6109,10 @@
       <c r="D3" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="121" t="s">
+      <c r="E3" s="119" t="s">
         <v>630</v>
       </c>
-      <c r="F3" s="121" t="s">
+      <c r="F3" s="119" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6163,8 +6129,8 @@
       <c r="D4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -6289,10 +6255,10 @@
       <c r="D11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="E11" s="119" t="s">
         <v>640</v>
       </c>
-      <c r="F11" s="121" t="s">
+      <c r="F11" s="119" t="s">
         <v>641</v>
       </c>
     </row>
@@ -6309,8 +6275,8 @@
       <c r="D12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="211.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -6325,8 +6291,8 @@
       <c r="D13" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -6451,10 +6417,10 @@
       <c r="D20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="121" t="s">
+      <c r="E20" s="119" t="s">
         <v>644</v>
       </c>
-      <c r="F20" s="121" t="s">
+      <c r="F20" s="119" t="s">
         <v>645</v>
       </c>
     </row>
@@ -6471,8 +6437,8 @@
       <c r="D21" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="121"/>
-      <c r="F21" s="121"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -7397,10 +7363,10 @@
       <c r="D70" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="121" t="s">
+      <c r="E70" s="119" t="s">
         <v>651</v>
       </c>
-      <c r="F70" s="121" t="s">
+      <c r="F70" s="119" t="s">
         <v>652</v>
       </c>
     </row>
@@ -7417,8 +7383,8 @@
       <c r="D71" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="121"/>
-      <c r="F71" s="121"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -7703,10 +7669,10 @@
       <c r="D86" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="114" t="s">
+      <c r="E86" s="116" t="s">
         <v>658</v>
       </c>
-      <c r="F86" s="114" t="s">
+      <c r="F86" s="116" t="s">
         <v>659</v>
       </c>
     </row>
@@ -7723,8 +7689,8 @@
       <c r="D87" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="114"/>
-      <c r="F87" s="114"/>
+      <c r="E87" s="116"/>
+      <c r="F87" s="116"/>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A88" s="24" t="s">
@@ -7739,8 +7705,8 @@
       <c r="D88" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="114"/>
-      <c r="F88" s="114"/>
+      <c r="E88" s="116"/>
+      <c r="F88" s="116"/>
     </row>
     <row r="89" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A89" s="24" t="s">
@@ -8225,10 +8191,10 @@
       <c r="D114" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="121" t="s">
+      <c r="E114" s="119" t="s">
         <v>662</v>
       </c>
-      <c r="F114" s="121" t="s">
+      <c r="F114" s="119" t="s">
         <v>308</v>
       </c>
     </row>
@@ -8245,8 +8211,8 @@
       <c r="D115" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="121"/>
-      <c r="F115" s="121"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="119"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -9009,10 +8975,10 @@
       <c r="D156" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="121" t="s">
+      <c r="E156" s="119" t="s">
         <v>681</v>
       </c>
-      <c r="F156" s="121" t="s">
+      <c r="F156" s="119" t="s">
         <v>657</v>
       </c>
     </row>
@@ -9029,8 +8995,8 @@
       <c r="D157" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="121"/>
-      <c r="F157" s="121"/>
+      <c r="E157" s="119"/>
+      <c r="F157" s="119"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
@@ -9234,6 +9200,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="A82:F82"/>
     <mergeCell ref="E156:E157"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="A91:F91"/>
@@ -9247,25 +9232,6 @@
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
     <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9478,10 +9444,10 @@
       <c r="D11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="114" t="s">
+      <c r="E11" s="116" t="s">
         <v>729</v>
       </c>
-      <c r="F11" s="115" t="s">
+      <c r="F11" s="117" t="s">
         <v>730</v>
       </c>
     </row>
@@ -9498,8 +9464,8 @@
       <c r="D12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="118"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -12451,14 +12417,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -12471,6 +12429,14 @@
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
     <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12683,10 +12649,10 @@
       <c r="D11" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="121" t="s">
         <v>735</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="121" t="s">
         <v>736</v>
       </c>
     </row>
@@ -12703,8 +12669,8 @@
       <c r="D12" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
     </row>
     <row r="13" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -12847,10 +12813,10 @@
       <c r="D20" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="121" t="s">
         <v>737</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="121" t="s">
         <v>738</v>
       </c>
     </row>
@@ -12867,8 +12833,8 @@
       <c r="D21" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -13793,10 +13759,10 @@
       <c r="D70" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="121" t="s">
         <v>745</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="121" t="s">
         <v>746</v>
       </c>
     </row>
@@ -13813,8 +13779,8 @@
       <c r="D71" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="122"/>
+      <c r="F71" s="122"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -15019,10 +14985,10 @@
       <c r="D135" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="119" t="s">
+      <c r="E135" s="121" t="s">
         <v>758</v>
       </c>
-      <c r="F135" s="119" t="s">
+      <c r="F135" s="121" t="s">
         <v>748</v>
       </c>
     </row>
@@ -15039,8 +15005,8 @@
       <c r="D136" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E136" s="120"/>
-      <c r="F136" s="120"/>
+      <c r="E136" s="122"/>
+      <c r="F136" s="122"/>
     </row>
     <row r="137" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A137" s="24" t="s">
@@ -15644,13 +15610,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A33:F33"/>
@@ -15665,11 +15629,13 @@
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A125:F125"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E135:E136"/>
-    <mergeCell ref="F135:F136"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15711,14 +15677,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -18071,10 +18037,10 @@
       <c r="D126" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="114" t="s">
+      <c r="E126" s="116" t="s">
         <v>469</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="117" t="s">
         <v>470</v>
       </c>
     </row>
@@ -18091,8 +18057,8 @@
       <c r="D127" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="114"/>
-      <c r="F127" s="116"/>
+      <c r="E127" s="116"/>
+      <c r="F127" s="118"/>
     </row>
     <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -18866,12 +18832,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -18884,6 +18844,12 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18947,10 +18913,10 @@
       <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="114" t="s">
+      <c r="E3" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="114" t="s">
+      <c r="F3" s="116" t="s">
         <v>28</v>
       </c>
     </row>
@@ -18967,8 +18933,8 @@
       <c r="D4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
     </row>
     <row r="5" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -19093,10 +19059,10 @@
       <c r="D11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="E11" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="121" t="s">
+      <c r="F11" s="119" t="s">
         <v>53</v>
       </c>
     </row>
@@ -19113,8 +19079,8 @@
       <c r="D12" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -19129,8 +19095,8 @@
       <c r="D13" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -20197,10 +20163,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="114" t="s">
+      <c r="E70" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="F70" s="114" t="s">
+      <c r="F70" s="116" t="s">
         <v>202</v>
       </c>
     </row>
@@ -20217,8 +20183,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
+      <c r="E71" s="116"/>
+      <c r="F71" s="116"/>
     </row>
     <row r="72" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -21033,10 +20999,10 @@
       <c r="D114" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="121" t="s">
+      <c r="E114" s="119" t="s">
         <v>307</v>
       </c>
-      <c r="F114" s="121" t="s">
+      <c r="F114" s="119" t="s">
         <v>308</v>
       </c>
     </row>
@@ -21053,8 +21019,8 @@
       <c r="D115" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="121"/>
-      <c r="F115" s="121"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="119"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -21259,10 +21225,10 @@
       <c r="D126" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="121" t="s">
+      <c r="E126" s="119" t="s">
         <v>335</v>
       </c>
-      <c r="F126" s="121" t="s">
+      <c r="F126" s="119" t="s">
         <v>336</v>
       </c>
     </row>
@@ -21279,8 +21245,8 @@
       <c r="D127" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="121"/>
-      <c r="F127" s="121"/>
+      <c r="E127" s="119"/>
+      <c r="F127" s="119"/>
     </row>
     <row r="128" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -21365,10 +21331,10 @@
       <c r="D132" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="121" t="s">
+      <c r="E132" s="119" t="s">
         <v>348</v>
       </c>
-      <c r="F132" s="121" t="s">
+      <c r="F132" s="119" t="s">
         <v>349</v>
       </c>
     </row>
@@ -21385,8 +21351,8 @@
       <c r="D133" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="121"/>
-      <c r="F133" s="121"/>
+      <c r="E133" s="119"/>
+      <c r="F133" s="119"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -21751,10 +21717,10 @@
       <c r="D152" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="122" t="s">
+      <c r="E152" s="120" t="s">
         <v>400</v>
       </c>
-      <c r="F152" s="122" t="s">
+      <c r="F152" s="120" t="s">
         <v>401</v>
       </c>
     </row>
@@ -21771,8 +21737,8 @@
       <c r="D153" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="122"/>
-      <c r="F153" s="122"/>
+      <c r="E153" s="120"/>
+      <c r="F153" s="120"/>
     </row>
     <row r="154" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
@@ -21817,10 +21783,10 @@
       <c r="D156" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="119" t="s">
+      <c r="E156" s="121" t="s">
         <v>410</v>
       </c>
-      <c r="F156" s="119" t="s">
+      <c r="F156" s="121" t="s">
         <v>411</v>
       </c>
     </row>
@@ -21837,8 +21803,8 @@
       <c r="D157" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="120"/>
-      <c r="F157" s="120"/>
+      <c r="E157" s="122"/>
+      <c r="F157" s="122"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
@@ -22042,22 +22008,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="E156:E157"/>
@@ -22074,6 +22024,22 @@
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -22146,10 +22112,10 @@
       <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="121" t="s">
+      <c r="E3" s="119" t="s">
         <v>482</v>
       </c>
-      <c r="F3" s="121" t="s">
+      <c r="F3" s="119" t="s">
         <v>483</v>
       </c>
     </row>
@@ -22166,8 +22132,8 @@
       <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -22292,10 +22258,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="E11" s="119" t="s">
         <v>487</v>
       </c>
-      <c r="F11" s="121" t="s">
+      <c r="F11" s="119" t="s">
         <v>488</v>
       </c>
     </row>
@@ -22312,8 +22278,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -22328,8 +22294,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -23293,10 +23259,10 @@
       <c r="D64" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="121" t="s">
+      <c r="E64" s="119" t="s">
         <v>504</v>
       </c>
-      <c r="F64" s="121" t="s">
+      <c r="F64" s="119" t="s">
         <v>505</v>
       </c>
     </row>
@@ -23313,8 +23279,8 @@
       <c r="D65" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="121"/>
-      <c r="F65" s="121"/>
+      <c r="E65" s="119"/>
+      <c r="F65" s="119"/>
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -23399,10 +23365,10 @@
       <c r="D70" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E70" s="121" t="s">
+      <c r="E70" s="119" t="s">
         <v>506</v>
       </c>
-      <c r="F70" s="121" t="s">
+      <c r="F70" s="119" t="s">
         <v>507</v>
       </c>
       <c r="G70" s="63"/>
@@ -23420,8 +23386,8 @@
       <c r="D71" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="121"/>
-      <c r="F71" s="121"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
       <c r="G71" s="63"/>
     </row>
     <row r="72" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -24239,10 +24205,10 @@
       <c r="D114" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="124" t="s">
+      <c r="E114" s="123" t="s">
         <v>513</v>
       </c>
-      <c r="F114" s="114" t="s">
+      <c r="F114" s="116" t="s">
         <v>514</v>
       </c>
     </row>
@@ -24259,8 +24225,8 @@
       <c r="D115" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="124"/>
-      <c r="F115" s="114"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="116"/>
     </row>
     <row r="116" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -24465,10 +24431,10 @@
       <c r="D126" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="114" t="s">
+      <c r="E126" s="116" t="s">
         <v>517</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="117" t="s">
         <v>518</v>
       </c>
     </row>
@@ -24485,8 +24451,8 @@
       <c r="D127" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="114"/>
-      <c r="F127" s="116"/>
+      <c r="E127" s="116"/>
+      <c r="F127" s="118"/>
     </row>
     <row r="128" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -24570,10 +24536,10 @@
       <c r="D132" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="114" t="s">
+      <c r="E132" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="F132" s="114" t="s">
+      <c r="F132" s="116" t="s">
         <v>520</v>
       </c>
     </row>
@@ -24590,8 +24556,8 @@
       <c r="D133" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="114"/>
-      <c r="F133" s="114"/>
+      <c r="E133" s="116"/>
+      <c r="F133" s="116"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -24606,8 +24572,8 @@
       <c r="D134" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="114"/>
-      <c r="F134" s="114"/>
+      <c r="E134" s="116"/>
+      <c r="F134" s="116"/>
     </row>
     <row r="135" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A135" s="24" t="s">
@@ -24775,7 +24741,7 @@
       <c r="E143" s="29" t="s">
         <v>521</v>
       </c>
-      <c r="F143" s="121" t="s">
+      <c r="F143" s="119" t="s">
         <v>379</v>
       </c>
     </row>
@@ -24795,7 +24761,7 @@
       <c r="E144" s="29" t="s">
         <v>522</v>
       </c>
-      <c r="F144" s="121"/>
+      <c r="F144" s="119"/>
     </row>
     <row r="145" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
@@ -24910,10 +24876,10 @@
       <c r="D150" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E150" s="115" t="s">
+      <c r="E150" s="117" t="s">
         <v>528</v>
       </c>
-      <c r="F150" s="115" t="s">
+      <c r="F150" s="117" t="s">
         <v>529</v>
       </c>
       <c r="G150" s="68"/>
@@ -24931,8 +24897,8 @@
       <c r="D151" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E151" s="116"/>
-      <c r="F151" s="116"/>
+      <c r="E151" s="118"/>
+      <c r="F151" s="118"/>
       <c r="G151" s="63"/>
     </row>
     <row r="152" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -24948,10 +24914,10 @@
       <c r="D152" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="123" t="s">
+      <c r="E152" s="124" t="s">
         <v>530</v>
       </c>
-      <c r="F152" s="123" t="s">
+      <c r="F152" s="124" t="s">
         <v>502</v>
       </c>
     </row>
@@ -24968,8 +24934,8 @@
       <c r="D153" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="123"/>
-      <c r="F153" s="123"/>
+      <c r="E153" s="124"/>
+      <c r="F153" s="124"/>
     </row>
     <row r="154" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
@@ -25243,12 +25209,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -25262,22 +25238,12 @@
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25341,10 +25307,10 @@
       <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="121" t="s">
+      <c r="E3" s="119" t="s">
         <v>532</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="121" t="s">
         <v>533</v>
       </c>
     </row>
@@ -25361,8 +25327,8 @@
       <c r="D4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -25487,10 +25453,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="121" t="s">
         <v>537</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="121" t="s">
         <v>538</v>
       </c>
     </row>
@@ -25507,8 +25473,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
     </row>
     <row r="13" spans="1:6" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -25523,8 +25489,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
     </row>
     <row r="14" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -26589,10 +26555,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="121" t="s">
         <v>548</v>
       </c>
-      <c r="F70" s="115" t="s">
+      <c r="F70" s="117" t="s">
         <v>549</v>
       </c>
     </row>
@@ -26609,8 +26575,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="126"/>
+      <c r="E71" s="122"/>
+      <c r="F71" s="128"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -27651,10 +27617,10 @@
       <c r="D126" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="114" t="s">
+      <c r="E126" s="116" t="s">
         <v>558</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="117" t="s">
         <v>559</v>
       </c>
     </row>
@@ -27671,8 +27637,8 @@
       <c r="D127" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="114"/>
-      <c r="F127" s="116"/>
+      <c r="E127" s="116"/>
+      <c r="F127" s="118"/>
     </row>
     <row r="128" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -27755,10 +27721,10 @@
       <c r="D132" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="114" t="s">
+      <c r="E132" s="116" t="s">
         <v>560</v>
       </c>
-      <c r="F132" s="115" t="s">
+      <c r="F132" s="117" t="s">
         <v>561</v>
       </c>
     </row>
@@ -27775,8 +27741,8 @@
       <c r="D133" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="114"/>
-      <c r="F133" s="116"/>
+      <c r="E133" s="116"/>
+      <c r="F133" s="118"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -28271,10 +28237,10 @@
       <c r="D159" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="127" t="s">
+      <c r="E159" s="125" t="s">
         <v>571</v>
       </c>
-      <c r="F159" s="128" t="s">
+      <c r="F159" s="126" t="s">
         <v>572</v>
       </c>
     </row>
@@ -28291,8 +28257,8 @@
       <c r="D160" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="127"/>
-      <c r="F160" s="129"/>
+      <c r="E160" s="125"/>
+      <c r="F160" s="127"/>
     </row>
     <row r="161" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A161" s="24" t="s">
@@ -28436,16 +28402,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -28458,23 +28420,27 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54373480-9F78-4E50-9D2A-7D7432A20250}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54373480-9F78-4E50-9D2A-7D7432A20250}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28676,10 +28642,10 @@
       <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="E11" s="119" t="s">
         <v>889</v>
       </c>
-      <c r="F11" s="121" t="s">
+      <c r="F11" s="119" t="s">
         <v>890</v>
       </c>
     </row>
@@ -28696,8 +28662,8 @@
       <c r="D12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -28842,10 +28808,10 @@
       <c r="D20" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="114" t="s">
+      <c r="E20" s="116" t="s">
         <v>895</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="116" t="s">
         <v>896</v>
       </c>
     </row>
@@ -28862,8 +28828,8 @@
       <c r="D21" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="116"/>
     </row>
     <row r="22" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -29526,10 +29492,10 @@
       <c r="D56" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="121" t="s">
+      <c r="E56" s="119" t="s">
         <v>907</v>
       </c>
-      <c r="F56" s="121" t="s">
+      <c r="F56" s="119" t="s">
         <v>908</v>
       </c>
     </row>
@@ -29546,8 +29512,8 @@
       <c r="D57" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="121"/>
-      <c r="F57" s="121"/>
+      <c r="E57" s="119"/>
+      <c r="F57" s="119"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
@@ -29782,10 +29748,10 @@
       <c r="D70" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="121" t="s">
+      <c r="E70" s="119" t="s">
         <v>911</v>
       </c>
-      <c r="F70" s="121" t="s">
+      <c r="F70" s="119" t="s">
         <v>912</v>
       </c>
     </row>
@@ -29802,8 +29768,8 @@
       <c r="D71" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="121"/>
-      <c r="F71" s="121"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -29858,10 +29824,10 @@
       <c r="D74" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="114" t="s">
+      <c r="E74" s="116" t="s">
         <v>913</v>
       </c>
-      <c r="F74" s="114" t="s">
+      <c r="F74" s="116" t="s">
         <v>914</v>
       </c>
     </row>
@@ -29878,8 +29844,8 @@
       <c r="D75" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="114"/>
-      <c r="F75" s="114"/>
+      <c r="E75" s="116"/>
+      <c r="F75" s="116"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -30214,10 +30180,10 @@
       <c r="D93" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="115" t="s">
+      <c r="E93" s="117" t="s">
         <v>919</v>
       </c>
-      <c r="F93" s="115" t="s">
+      <c r="F93" s="117" t="s">
         <v>920</v>
       </c>
     </row>
@@ -30234,8 +30200,8 @@
       <c r="D94" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="116"/>
-      <c r="F94" s="116"/>
+      <c r="E94" s="118"/>
+      <c r="F94" s="118"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
@@ -30610,10 +30576,10 @@
       <c r="D114" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="114" t="s">
+      <c r="E114" s="116" t="s">
         <v>929</v>
       </c>
-      <c r="F114" s="114" t="s">
+      <c r="F114" s="116" t="s">
         <v>930</v>
       </c>
     </row>
@@ -30630,8 +30596,8 @@
       <c r="D115" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="114"/>
-      <c r="F115" s="114"/>
+      <c r="E115" s="116"/>
+      <c r="F115" s="116"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -31175,7 +31141,7 @@
       <c r="E144" s="86" t="s">
         <v>946</v>
       </c>
-      <c r="F144" s="121" t="s">
+      <c r="F144" s="119" t="s">
         <v>40</v>
       </c>
     </row>
@@ -31195,7 +31161,7 @@
       <c r="E145" s="86" t="s">
         <v>947</v>
       </c>
-      <c r="F145" s="121"/>
+      <c r="F145" s="119"/>
     </row>
     <row r="146" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
@@ -31619,6 +31585,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -31632,31 +31620,9 @@
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="E56:E57"/>
     <mergeCell ref="F56:F57"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F144:F145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31664,7 +31630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4716598-4E81-47BF-9B1B-F47650125005}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:F44"/>
     </sheetView>
   </sheetViews>
@@ -31868,10 +31834,10 @@
       <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="121" t="s">
         <v>835</v>
       </c>
-      <c r="F11" s="121" t="s">
+      <c r="F11" s="119" t="s">
         <v>836</v>
       </c>
     </row>
@@ -31888,8 +31854,8 @@
       <c r="D12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="120"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -32034,10 +32000,10 @@
       <c r="D20" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="114" t="s">
+      <c r="E20" s="116" t="s">
         <v>970</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="116" t="s">
         <v>971</v>
       </c>
     </row>
@@ -32054,8 +32020,8 @@
       <c r="D21" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="116"/>
     </row>
     <row r="22" spans="1:6" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -32980,10 +32946,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="121" t="s">
         <v>848</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="121" t="s">
         <v>849</v>
       </c>
     </row>
@@ -33000,8 +32966,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="122"/>
+      <c r="F71" s="122"/>
     </row>
     <row r="72" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -33056,10 +33022,10 @@
       <c r="D74" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="115" t="s">
+      <c r="E74" s="117" t="s">
         <v>852</v>
       </c>
-      <c r="F74" s="115" t="s">
+      <c r="F74" s="117" t="s">
         <v>851</v>
       </c>
     </row>
@@ -33076,8 +33042,8 @@
       <c r="D75" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="116"/>
-      <c r="F75" s="116"/>
+      <c r="E75" s="118"/>
+      <c r="F75" s="118"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -33812,10 +33778,10 @@
       <c r="D114" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="114" t="s">
+      <c r="E114" s="116" t="s">
         <v>861</v>
       </c>
-      <c r="F114" s="115" t="s">
+      <c r="F114" s="117" t="s">
         <v>862</v>
       </c>
     </row>
@@ -33832,8 +33798,8 @@
       <c r="D115" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="114"/>
-      <c r="F115" s="116"/>
+      <c r="E115" s="116"/>
+      <c r="F115" s="118"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -34827,26 +34793,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E74:E75"/>
     <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F114:F115"/>
@@ -34857,6 +34803,26 @@
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="F70:F71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -34920,10 +34886,10 @@
       <c r="D3" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="121" t="s">
+      <c r="E3" s="119" t="s">
         <v>767</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="121" t="s">
         <v>768</v>
       </c>
     </row>
@@ -34940,8 +34906,8 @@
       <c r="D4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -35066,10 +35032,10 @@
       <c r="D11" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="121" t="s">
         <v>773</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="121" t="s">
         <v>774</v>
       </c>
     </row>
@@ -35086,8 +35052,8 @@
       <c r="D12" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -35102,8 +35068,8 @@
       <c r="D13" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
     </row>
     <row r="14" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -35228,10 +35194,10 @@
       <c r="D20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="121" t="s">
+      <c r="E20" s="119" t="s">
         <v>777</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="121" t="s">
         <v>778</v>
       </c>
     </row>
@@ -35248,8 +35214,8 @@
       <c r="D21" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="121"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -36064,10 +36030,10 @@
       <c r="D64" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="119" t="s">
+      <c r="E64" s="121" t="s">
         <v>789</v>
       </c>
-      <c r="F64" s="119" t="s">
+      <c r="F64" s="121" t="s">
         <v>790</v>
       </c>
     </row>
@@ -36084,8 +36050,8 @@
       <c r="D65" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="120"/>
-      <c r="F65" s="120"/>
+      <c r="E65" s="122"/>
+      <c r="F65" s="122"/>
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -36170,10 +36136,10 @@
       <c r="D70" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="121" t="s">
+      <c r="E70" s="119" t="s">
         <v>791</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="121" t="s">
         <v>792</v>
       </c>
     </row>
@@ -36190,8 +36156,8 @@
       <c r="D71" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="121"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="122"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -36246,10 +36212,10 @@
       <c r="D74" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="119" t="s">
+      <c r="E74" s="121" t="s">
         <v>793</v>
       </c>
-      <c r="F74" s="125" t="s">
+      <c r="F74" s="129" t="s">
         <v>211</v>
       </c>
     </row>
@@ -36266,8 +36232,8 @@
       <c r="D75" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="120"/>
-      <c r="F75" s="120"/>
+      <c r="E75" s="122"/>
+      <c r="F75" s="122"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -37002,10 +36968,10 @@
       <c r="D114" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="119" t="s">
+      <c r="E114" s="121" t="s">
         <v>804</v>
       </c>
-      <c r="F114" s="119" t="s">
+      <c r="F114" s="121" t="s">
         <v>805</v>
       </c>
     </row>
@@ -37022,8 +36988,8 @@
       <c r="D115" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="120"/>
-      <c r="F115" s="120"/>
+      <c r="E115" s="122"/>
+      <c r="F115" s="122"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -38019,14 +37985,13 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E20:E21"/>
@@ -38036,11 +38001,14 @@
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="F70:F71"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
@@ -38049,8 +38017,6 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="E126:E127"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38115,10 +38081,10 @@
       <c r="D3" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="119" t="s">
+      <c r="E3" s="121" t="s">
         <v>575</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="121" t="s">
         <v>576</v>
       </c>
     </row>
@@ -38135,8 +38101,8 @@
       <c r="D4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -38261,10 +38227,10 @@
       <c r="D11" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="121" t="s">
         <v>584</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="121" t="s">
         <v>585</v>
       </c>
     </row>
@@ -38281,8 +38247,8 @@
       <c r="D12" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
     </row>
     <row r="13" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -38297,8 +38263,8 @@
       <c r="D13" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -38313,8 +38279,8 @@
       <c r="D14" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
@@ -38419,10 +38385,10 @@
       <c r="D20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="121" t="s">
         <v>586</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="121" t="s">
         <v>587</v>
       </c>
     </row>
@@ -38439,8 +38405,8 @@
       <c r="D21" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -39363,10 +39329,10 @@
       <c r="D70" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="121" t="s">
         <v>595</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="121" t="s">
         <v>596</v>
       </c>
     </row>
@@ -39383,8 +39349,8 @@
       <c r="D71" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="122"/>
+      <c r="F71" s="122"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -39439,10 +39405,10 @@
       <c r="D74" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="114" t="s">
+      <c r="E74" s="116" t="s">
         <v>598</v>
       </c>
-      <c r="F74" s="114" t="s">
+      <c r="F74" s="116" t="s">
         <v>598</v>
       </c>
     </row>
@@ -39459,8 +39425,8 @@
       <c r="D75" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="114"/>
-      <c r="F75" s="114"/>
+      <c r="E75" s="116"/>
+      <c r="F75" s="116"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -39793,10 +39759,10 @@
       <c r="D93" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="119" t="s">
+      <c r="E93" s="121" t="s">
         <v>606</v>
       </c>
-      <c r="F93" s="119" t="s">
+      <c r="F93" s="121" t="s">
         <v>593</v>
       </c>
     </row>
@@ -39813,8 +39779,8 @@
       <c r="D94" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="120"/>
-      <c r="F94" s="120"/>
+      <c r="E94" s="122"/>
+      <c r="F94" s="122"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
@@ -40189,10 +40155,10 @@
       <c r="D114" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="121" t="s">
+      <c r="E114" s="119" t="s">
         <v>613</v>
       </c>
-      <c r="F114" s="119" t="s">
+      <c r="F114" s="121" t="s">
         <v>614</v>
       </c>
     </row>
@@ -40209,8 +40175,8 @@
       <c r="D115" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="121"/>
-      <c r="F115" s="120"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="122"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -41206,14 +41172,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -41226,18 +41196,14 @@
     <mergeCell ref="E93:E94"/>
     <mergeCell ref="F93:F94"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
update and clean make_results.R and make.R
</commit_message>
<xml_diff>
--- a/rawdata/supplementary_material_V3.xlsx
+++ b/rawdata/supplementary_material_V3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F757ADB8-4269-444F-98CB-1E337A3411CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF0DDA7-0ECA-4826-8F74-98BCFEA33593}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="859" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="859" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring system" sheetId="1" r:id="rId1"/>
@@ -4914,12 +4914,6 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4929,11 +4923,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4941,13 +4935,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5403,10 +5403,10 @@
       <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="113" t="s">
         <v>938</v>
       </c>
-      <c r="F3" s="111" t="s">
+      <c r="F3" s="113" t="s">
         <v>604</v>
       </c>
     </row>
@@ -5423,8 +5423,8 @@
       <c r="D4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -5549,10 +5549,10 @@
       <c r="D11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="111" t="s">
+      <c r="E11" s="113" t="s">
         <v>612</v>
       </c>
-      <c r="F11" s="111" t="s">
+      <c r="F11" s="113" t="s">
         <v>613</v>
       </c>
     </row>
@@ -5569,8 +5569,8 @@
       <c r="D12" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -5585,8 +5585,8 @@
       <c r="D13" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -5711,10 +5711,10 @@
       <c r="D20" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="111" t="s">
+      <c r="E20" s="113" t="s">
         <v>616</v>
       </c>
-      <c r="F20" s="111" t="s">
+      <c r="F20" s="113" t="s">
         <v>617</v>
       </c>
     </row>
@@ -5731,8 +5731,8 @@
       <c r="D21" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -6655,10 +6655,10 @@
       <c r="D70" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="111" t="s">
+      <c r="E70" s="113" t="s">
         <v>623</v>
       </c>
-      <c r="F70" s="111" t="s">
+      <c r="F70" s="113" t="s">
         <v>624</v>
       </c>
     </row>
@@ -6675,8 +6675,8 @@
       <c r="D71" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="111"/>
-      <c r="F71" s="111"/>
+      <c r="E71" s="113"/>
+      <c r="F71" s="113"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -6961,10 +6961,10 @@
       <c r="D86" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="108" t="s">
+      <c r="E86" s="106" t="s">
         <v>630</v>
       </c>
-      <c r="F86" s="108" t="s">
+      <c r="F86" s="106" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6981,8 +6981,8 @@
       <c r="D87" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="108"/>
-      <c r="F87" s="108"/>
+      <c r="E87" s="106"/>
+      <c r="F87" s="106"/>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A88" s="24" t="s">
@@ -6997,8 +6997,8 @@
       <c r="D88" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="108"/>
-      <c r="F88" s="108"/>
+      <c r="E88" s="106"/>
+      <c r="F88" s="106"/>
     </row>
     <row r="89" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A89" s="24" t="s">
@@ -7483,10 +7483,10 @@
       <c r="D114" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="111" t="s">
+      <c r="E114" s="113" t="s">
         <v>634</v>
       </c>
-      <c r="F114" s="111" t="s">
+      <c r="F114" s="113" t="s">
         <v>298</v>
       </c>
     </row>
@@ -7503,8 +7503,8 @@
       <c r="D115" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="111"/>
-      <c r="F115" s="111"/>
+      <c r="E115" s="113"/>
+      <c r="F115" s="113"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -8267,10 +8267,10 @@
       <c r="D156" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="111" t="s">
+      <c r="E156" s="113" t="s">
         <v>653</v>
       </c>
-      <c r="F156" s="111" t="s">
+      <c r="F156" s="113" t="s">
         <v>629</v>
       </c>
     </row>
@@ -8287,8 +8287,8 @@
       <c r="D157" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="111"/>
-      <c r="F157" s="111"/>
+      <c r="E157" s="113"/>
+      <c r="F157" s="113"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
@@ -8492,12 +8492,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E156:E157"/>
+    <mergeCell ref="F156:F157"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
     <mergeCell ref="E86:E88"/>
     <mergeCell ref="F86:F88"/>
     <mergeCell ref="A19:F19"/>
@@ -8511,19 +8518,12 @@
     <mergeCell ref="E70:E71"/>
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
-    <mergeCell ref="E156:E157"/>
-    <mergeCell ref="F156:F157"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8534,7 +8534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA8B1E2-51E2-4ACA-A73C-C2AA2101D6A9}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -8737,10 +8737,10 @@
       <c r="D11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="108" t="s">
+      <c r="E11" s="106" t="s">
         <v>698</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="107" t="s">
         <v>699</v>
       </c>
     </row>
@@ -8757,8 +8757,8 @@
       <c r="D12" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="108"/>
-      <c r="F12" s="110"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -9971,10 +9971,10 @@
       <c r="D76" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="113" t="s">
+      <c r="E76" s="111" t="s">
         <v>674</v>
       </c>
-      <c r="F76" s="113" t="s">
+      <c r="F76" s="111" t="s">
         <v>675</v>
       </c>
     </row>
@@ -9991,8 +9991,8 @@
       <c r="D77" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="114"/>
-      <c r="F77" s="114"/>
+      <c r="E77" s="112"/>
+      <c r="F77" s="112"/>
     </row>
     <row r="78" spans="1:6" ht="195" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
@@ -11704,6 +11704,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -11718,14 +11726,6 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="E76:E77"/>
     <mergeCell ref="F76:F77"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11938,10 +11938,10 @@
       <c r="D11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="111" t="s">
         <v>704</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="111" t="s">
         <v>950</v>
       </c>
     </row>
@@ -11958,8 +11958,8 @@
       <c r="D12" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
     </row>
     <row r="13" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -12102,10 +12102,10 @@
       <c r="D20" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="113" t="s">
+      <c r="E20" s="111" t="s">
         <v>705</v>
       </c>
-      <c r="F20" s="113" t="s">
+      <c r="F20" s="111" t="s">
         <v>706</v>
       </c>
     </row>
@@ -12122,8 +12122,8 @@
       <c r="D21" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -13048,10 +13048,10 @@
       <c r="D70" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="113" t="s">
+      <c r="E70" s="111" t="s">
         <v>713</v>
       </c>
-      <c r="F70" s="113" t="s">
+      <c r="F70" s="111" t="s">
         <v>714</v>
       </c>
     </row>
@@ -13068,8 +13068,8 @@
       <c r="D71" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="112"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -14274,10 +14274,10 @@
       <c r="D135" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="113" t="s">
+      <c r="E135" s="111" t="s">
         <v>725</v>
       </c>
-      <c r="F135" s="113" t="s">
+      <c r="F135" s="111" t="s">
         <v>715</v>
       </c>
     </row>
@@ -14294,8 +14294,8 @@
       <c r="D136" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E136" s="114"/>
-      <c r="F136" s="114"/>
+      <c r="E136" s="112"/>
+      <c r="F136" s="112"/>
     </row>
     <row r="137" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A137" s="24" t="s">
@@ -14904,11 +14904,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E135:E136"/>
-    <mergeCell ref="F135:F136"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A33:F33"/>
@@ -14923,13 +14925,11 @@
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14971,14 +14971,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -17331,10 +17331,10 @@
       <c r="D126" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="108" t="s">
+      <c r="E126" s="106" t="s">
         <v>455</v>
       </c>
-      <c r="F126" s="109" t="s">
+      <c r="F126" s="107" t="s">
         <v>456</v>
       </c>
     </row>
@@ -17351,8 +17351,8 @@
       <c r="D127" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="108"/>
-      <c r="F127" s="110"/>
+      <c r="E127" s="106"/>
+      <c r="F127" s="108"/>
     </row>
     <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -18126,6 +18126,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -18138,12 +18144,6 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18153,7 +18153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6535A64-0113-4925-BB3F-009252BF36D5}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
@@ -18207,10 +18207,10 @@
       <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="108" t="s">
+      <c r="E3" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="F3" s="108" t="s">
+      <c r="F3" s="106" t="s">
         <v>936</v>
       </c>
     </row>
@@ -18227,8 +18227,8 @@
       <c r="D4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
     </row>
     <row r="5" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -18353,10 +18353,10 @@
       <c r="D11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="111" t="s">
+      <c r="F11" s="113" t="s">
         <v>945</v>
       </c>
     </row>
@@ -18373,8 +18373,8 @@
       <c r="D12" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
     </row>
     <row r="13" spans="1:6" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -18389,8 +18389,8 @@
       <c r="D13" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
     </row>
     <row r="14" spans="1:6" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -19457,10 +19457,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="108" t="s">
+      <c r="E70" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="F70" s="108" t="s">
+      <c r="F70" s="106" t="s">
         <v>193</v>
       </c>
     </row>
@@ -19477,8 +19477,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="108"/>
-      <c r="F71" s="108"/>
+      <c r="E71" s="106"/>
+      <c r="F71" s="106"/>
     </row>
     <row r="72" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -20293,10 +20293,10 @@
       <c r="D114" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="111" t="s">
+      <c r="E114" s="113" t="s">
         <v>297</v>
       </c>
-      <c r="F114" s="111" t="s">
+      <c r="F114" s="113" t="s">
         <v>298</v>
       </c>
     </row>
@@ -20313,8 +20313,8 @@
       <c r="D115" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="111"/>
-      <c r="F115" s="111"/>
+      <c r="E115" s="113"/>
+      <c r="F115" s="113"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -20519,10 +20519,10 @@
       <c r="D126" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="111" t="s">
+      <c r="E126" s="113" t="s">
         <v>324</v>
       </c>
-      <c r="F126" s="111" t="s">
+      <c r="F126" s="113" t="s">
         <v>325</v>
       </c>
     </row>
@@ -20539,8 +20539,8 @@
       <c r="D127" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="111"/>
-      <c r="F127" s="111"/>
+      <c r="E127" s="113"/>
+      <c r="F127" s="113"/>
     </row>
     <row r="128" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -20625,10 +20625,10 @@
       <c r="D132" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="111" t="s">
+      <c r="E132" s="113" t="s">
         <v>337</v>
       </c>
-      <c r="F132" s="111" t="s">
+      <c r="F132" s="113" t="s">
         <v>338</v>
       </c>
     </row>
@@ -20645,8 +20645,8 @@
       <c r="D133" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="111"/>
-      <c r="F133" s="111"/>
+      <c r="E133" s="113"/>
+      <c r="F133" s="113"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -21011,10 +21011,10 @@
       <c r="D152" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="112" t="s">
+      <c r="E152" s="115" t="s">
         <v>389</v>
       </c>
-      <c r="F152" s="112" t="s">
+      <c r="F152" s="115" t="s">
         <v>390</v>
       </c>
     </row>
@@ -21031,8 +21031,8 @@
       <c r="D153" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="112"/>
-      <c r="F153" s="112"/>
+      <c r="E153" s="115"/>
+      <c r="F153" s="115"/>
     </row>
     <row r="154" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
@@ -21077,10 +21077,10 @@
       <c r="D156" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="113" t="s">
+      <c r="E156" s="111" t="s">
         <v>399</v>
       </c>
-      <c r="F156" s="113" t="s">
+      <c r="F156" s="111" t="s">
         <v>400</v>
       </c>
     </row>
@@ -21097,8 +21097,8 @@
       <c r="D157" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="114"/>
-      <c r="F157" s="114"/>
+      <c r="E157" s="112"/>
+      <c r="F157" s="112"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
@@ -21302,6 +21302,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="E156:E157"/>
@@ -21318,22 +21334,6 @@
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -21405,10 +21405,10 @@
       <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="113" t="s">
         <v>937</v>
       </c>
-      <c r="F3" s="111" t="s">
+      <c r="F3" s="113" t="s">
         <v>468</v>
       </c>
     </row>
@@ -21425,8 +21425,8 @@
       <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -21551,10 +21551,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="111" t="s">
+      <c r="E11" s="113" t="s">
         <v>472</v>
       </c>
-      <c r="F11" s="111" t="s">
+      <c r="F11" s="113" t="s">
         <v>473</v>
       </c>
     </row>
@@ -21571,8 +21571,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -21587,8 +21587,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -22552,10 +22552,10 @@
       <c r="D64" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="111" t="s">
+      <c r="E64" s="113" t="s">
         <v>489</v>
       </c>
-      <c r="F64" s="111" t="s">
+      <c r="F64" s="113" t="s">
         <v>490</v>
       </c>
     </row>
@@ -22572,8 +22572,8 @@
       <c r="D65" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="111"/>
-      <c r="F65" s="111"/>
+      <c r="E65" s="113"/>
+      <c r="F65" s="113"/>
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -22658,10 +22658,10 @@
       <c r="D70" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E70" s="111" t="s">
+      <c r="E70" s="113" t="s">
         <v>964</v>
       </c>
-      <c r="F70" s="111" t="s">
+      <c r="F70" s="113" t="s">
         <v>965</v>
       </c>
       <c r="G70" s="62"/>
@@ -22679,8 +22679,8 @@
       <c r="D71" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="111"/>
-      <c r="F71" s="111"/>
+      <c r="E71" s="113"/>
+      <c r="F71" s="113"/>
       <c r="G71" s="62"/>
     </row>
     <row r="72" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -23498,10 +23498,10 @@
       <c r="D114" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="116" t="s">
+      <c r="E114" s="117" t="s">
         <v>494</v>
       </c>
-      <c r="F114" s="108" t="s">
+      <c r="F114" s="106" t="s">
         <v>495</v>
       </c>
     </row>
@@ -23518,8 +23518,8 @@
       <c r="D115" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="116"/>
-      <c r="F115" s="108"/>
+      <c r="E115" s="117"/>
+      <c r="F115" s="106"/>
     </row>
     <row r="116" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -23724,10 +23724,10 @@
       <c r="D126" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="108" t="s">
+      <c r="E126" s="106" t="s">
         <v>498</v>
       </c>
-      <c r="F126" s="109" t="s">
+      <c r="F126" s="107" t="s">
         <v>499</v>
       </c>
     </row>
@@ -23744,8 +23744,8 @@
       <c r="D127" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="108"/>
-      <c r="F127" s="110"/>
+      <c r="E127" s="106"/>
+      <c r="F127" s="108"/>
     </row>
     <row r="128" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -23829,10 +23829,10 @@
       <c r="D132" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="108" t="s">
+      <c r="E132" s="106" t="s">
         <v>500</v>
       </c>
-      <c r="F132" s="108" t="s">
+      <c r="F132" s="106" t="s">
         <v>501</v>
       </c>
     </row>
@@ -23849,8 +23849,8 @@
       <c r="D133" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="108"/>
-      <c r="F133" s="108"/>
+      <c r="E133" s="106"/>
+      <c r="F133" s="106"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -23865,8 +23865,8 @@
       <c r="D134" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="108"/>
-      <c r="F134" s="108"/>
+      <c r="E134" s="106"/>
+      <c r="F134" s="106"/>
     </row>
     <row r="135" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A135" s="24" t="s">
@@ -24034,7 +24034,7 @@
       <c r="E143" s="29" t="s">
         <v>502</v>
       </c>
-      <c r="F143" s="111" t="s">
+      <c r="F143" s="113" t="s">
         <v>368</v>
       </c>
     </row>
@@ -24054,7 +24054,7 @@
       <c r="E144" s="29" t="s">
         <v>503</v>
       </c>
-      <c r="F144" s="111"/>
+      <c r="F144" s="113"/>
     </row>
     <row r="145" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
@@ -24169,10 +24169,10 @@
       <c r="D150" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E150" s="109" t="s">
+      <c r="E150" s="107" t="s">
         <v>509</v>
       </c>
-      <c r="F150" s="109" t="s">
+      <c r="F150" s="107" t="s">
         <v>510</v>
       </c>
       <c r="G150" s="66"/>
@@ -24190,8 +24190,8 @@
       <c r="D151" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E151" s="110"/>
-      <c r="F151" s="110"/>
+      <c r="E151" s="108"/>
+      <c r="F151" s="108"/>
       <c r="G151" s="62"/>
     </row>
     <row r="152" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -24207,10 +24207,10 @@
       <c r="D152" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="117" t="s">
+      <c r="E152" s="116" t="s">
         <v>511</v>
       </c>
-      <c r="F152" s="117" t="s">
+      <c r="F152" s="116" t="s">
         <v>487</v>
       </c>
     </row>
@@ -24227,8 +24227,8 @@
       <c r="D153" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="117"/>
-      <c r="F153" s="117"/>
+      <c r="E153" s="116"/>
+      <c r="F153" s="116"/>
     </row>
     <row r="154" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
@@ -24502,22 +24502,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -24531,12 +24521,22 @@
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24600,10 +24600,10 @@
       <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="113" t="s">
         <v>513</v>
       </c>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="111" t="s">
         <v>514</v>
       </c>
     </row>
@@ -24620,8 +24620,8 @@
       <c r="D4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="114"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="112"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -24746,10 +24746,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="111" t="s">
         <v>518</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="111" t="s">
         <v>519</v>
       </c>
     </row>
@@ -24766,8 +24766,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
     </row>
     <row r="13" spans="1:6" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -24782,8 +24782,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
     </row>
     <row r="14" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -25848,10 +25848,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="113" t="s">
+      <c r="E70" s="111" t="s">
         <v>529</v>
       </c>
-      <c r="F70" s="109" t="s">
+      <c r="F70" s="107" t="s">
         <v>530</v>
       </c>
     </row>
@@ -25868,7 +25868,7 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="114"/>
+      <c r="E71" s="112"/>
       <c r="F71" s="118"/>
     </row>
     <row r="72" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -26910,10 +26910,10 @@
       <c r="D126" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="108" t="s">
+      <c r="E126" s="106" t="s">
         <v>537</v>
       </c>
-      <c r="F126" s="109" t="s">
+      <c r="F126" s="107" t="s">
         <v>538</v>
       </c>
     </row>
@@ -26930,8 +26930,8 @@
       <c r="D127" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="108"/>
-      <c r="F127" s="110"/>
+      <c r="E127" s="106"/>
+      <c r="F127" s="108"/>
     </row>
     <row r="128" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
@@ -27014,10 +27014,10 @@
       <c r="D132" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="108" t="s">
+      <c r="E132" s="106" t="s">
         <v>539</v>
       </c>
-      <c r="F132" s="109" t="s">
+      <c r="F132" s="107" t="s">
         <v>540</v>
       </c>
     </row>
@@ -27034,8 +27034,8 @@
       <c r="D133" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="108"/>
-      <c r="F133" s="110"/>
+      <c r="E133" s="106"/>
+      <c r="F133" s="108"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
@@ -27530,10 +27530,10 @@
       <c r="D159" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="108" t="s">
+      <c r="E159" s="106" t="s">
         <v>550</v>
       </c>
-      <c r="F159" s="109" t="s">
+      <c r="F159" s="107" t="s">
         <v>999</v>
       </c>
     </row>
@@ -27550,8 +27550,8 @@
       <c r="D160" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="108"/>
-      <c r="F160" s="110"/>
+      <c r="E160" s="106"/>
+      <c r="F160" s="108"/>
     </row>
     <row r="161" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A161" s="24" t="s">
@@ -27695,12 +27695,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -27713,16 +27717,12 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27935,10 +27935,10 @@
       <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="111" t="s">
+      <c r="E11" s="113" t="s">
         <v>922</v>
       </c>
-      <c r="F11" s="111" t="s">
+      <c r="F11" s="113" t="s">
         <v>851</v>
       </c>
     </row>
@@ -27955,8 +27955,8 @@
       <c r="D12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="150.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -28101,10 +28101,10 @@
       <c r="D20" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="108" t="s">
+      <c r="E20" s="106" t="s">
         <v>856</v>
       </c>
-      <c r="F20" s="108" t="s">
+      <c r="F20" s="106" t="s">
         <v>857</v>
       </c>
     </row>
@@ -28121,8 +28121,8 @@
       <c r="D21" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
     </row>
     <row r="22" spans="1:6" ht="200.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -28785,10 +28785,10 @@
       <c r="D56" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="111" t="s">
+      <c r="E56" s="113" t="s">
         <v>863</v>
       </c>
-      <c r="F56" s="111" t="s">
+      <c r="F56" s="113" t="s">
         <v>864</v>
       </c>
     </row>
@@ -28805,8 +28805,8 @@
       <c r="D57" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="111"/>
-      <c r="F57" s="111"/>
+      <c r="E57" s="113"/>
+      <c r="F57" s="113"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
@@ -29041,10 +29041,10 @@
       <c r="D70" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="111" t="s">
+      <c r="E70" s="113" t="s">
         <v>926</v>
       </c>
-      <c r="F70" s="111" t="s">
+      <c r="F70" s="113" t="s">
         <v>1006</v>
       </c>
     </row>
@@ -29061,8 +29061,8 @@
       <c r="D71" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="111"/>
-      <c r="F71" s="111"/>
+      <c r="E71" s="113"/>
+      <c r="F71" s="113"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -29117,10 +29117,10 @@
       <c r="D74" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="108" t="s">
+      <c r="E74" s="106" t="s">
         <v>987</v>
       </c>
-      <c r="F74" s="108" t="s">
+      <c r="F74" s="106" t="s">
         <v>867</v>
       </c>
     </row>
@@ -29137,8 +29137,8 @@
       <c r="D75" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="108"/>
-      <c r="F75" s="108"/>
+      <c r="E75" s="106"/>
+      <c r="F75" s="106"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -29473,10 +29473,10 @@
       <c r="D93" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="109" t="s">
+      <c r="E93" s="107" t="s">
         <v>871</v>
       </c>
-      <c r="F93" s="109" t="s">
+      <c r="F93" s="107" t="s">
         <v>872</v>
       </c>
     </row>
@@ -29493,8 +29493,8 @@
       <c r="D94" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="110"/>
-      <c r="F94" s="110"/>
+      <c r="E94" s="108"/>
+      <c r="F94" s="108"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
@@ -29869,10 +29869,10 @@
       <c r="D114" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="108" t="s">
+      <c r="E114" s="106" t="s">
         <v>880</v>
       </c>
-      <c r="F114" s="108" t="s">
+      <c r="F114" s="106" t="s">
         <v>881</v>
       </c>
     </row>
@@ -29889,8 +29889,8 @@
       <c r="D115" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="108"/>
-      <c r="F115" s="108"/>
+      <c r="E115" s="106"/>
+      <c r="F115" s="106"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -30434,7 +30434,7 @@
       <c r="E144" s="92" t="s">
         <v>894</v>
       </c>
-      <c r="F144" s="111" t="s">
+      <c r="F144" s="113" t="s">
         <v>38</v>
       </c>
     </row>
@@ -30454,7 +30454,7 @@
       <c r="E145" s="92" t="s">
         <v>895</v>
       </c>
-      <c r="F145" s="111"/>
+      <c r="F145" s="113"/>
     </row>
     <row r="146" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
@@ -30882,15 +30882,19 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="F114:F115"/>
     <mergeCell ref="A69:F69"/>
@@ -30904,19 +30908,15 @@
     <mergeCell ref="F93:F94"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F144:F145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31131,10 +31131,10 @@
       <c r="D11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="111" t="s">
         <v>801</v>
       </c>
-      <c r="F11" s="111" t="s">
+      <c r="F11" s="113" t="s">
         <v>802</v>
       </c>
     </row>
@@ -31151,8 +31151,8 @@
       <c r="D12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="111"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="113"/>
     </row>
     <row r="13" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -31297,10 +31297,10 @@
       <c r="D20" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="108" t="s">
+      <c r="E20" s="106" t="s">
         <v>915</v>
       </c>
-      <c r="F20" s="108" t="s">
+      <c r="F20" s="106" t="s">
         <v>952</v>
       </c>
     </row>
@@ -31317,8 +31317,8 @@
       <c r="D21" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
     </row>
     <row r="22" spans="1:6" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -31981,10 +31981,10 @@
       <c r="D56" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="113" t="s">
+      <c r="E56" s="111" t="s">
         <v>913</v>
       </c>
-      <c r="F56" s="113" t="s">
+      <c r="F56" s="111" t="s">
         <v>914</v>
       </c>
     </row>
@@ -32001,8 +32001,8 @@
       <c r="D57" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="114"/>
-      <c r="F57" s="114"/>
+      <c r="E57" s="112"/>
+      <c r="F57" s="112"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
@@ -32237,10 +32237,10 @@
       <c r="D70" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="113" t="s">
+      <c r="E70" s="111" t="s">
         <v>814</v>
       </c>
-      <c r="F70" s="113" t="s">
+      <c r="F70" s="111" t="s">
         <v>815</v>
       </c>
     </row>
@@ -32257,8 +32257,8 @@
       <c r="D71" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="112"/>
     </row>
     <row r="72" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -32313,10 +32313,10 @@
       <c r="D74" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="109" t="s">
+      <c r="E74" s="107" t="s">
         <v>817</v>
       </c>
-      <c r="F74" s="109" t="s">
+      <c r="F74" s="107" t="s">
         <v>816</v>
       </c>
     </row>
@@ -32333,8 +32333,8 @@
       <c r="D75" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="110"/>
-      <c r="F75" s="110"/>
+      <c r="E75" s="108"/>
+      <c r="F75" s="108"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -33069,10 +33069,10 @@
       <c r="D114" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="108" t="s">
+      <c r="E114" s="106" t="s">
         <v>826</v>
       </c>
-      <c r="F114" s="109" t="s">
+      <c r="F114" s="107" t="s">
         <v>827</v>
       </c>
     </row>
@@ -33089,8 +33089,8 @@
       <c r="D115" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="108"/>
-      <c r="F115" s="110"/>
+      <c r="E115" s="106"/>
+      <c r="F115" s="108"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -34084,6 +34084,28 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E74:E75"/>
     <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F114:F115"/>
@@ -34094,28 +34116,6 @@
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34179,10 +34179,10 @@
       <c r="D3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="113" t="s">
         <v>734</v>
       </c>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="111" t="s">
         <v>735</v>
       </c>
     </row>
@@ -34199,8 +34199,8 @@
       <c r="D4" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="111"/>
-      <c r="F4" s="114"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="112"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -34325,10 +34325,10 @@
       <c r="D11" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="111" t="s">
         <v>946</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="111" t="s">
         <v>740</v>
       </c>
     </row>
@@ -34345,8 +34345,8 @@
       <c r="D12" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -34361,8 +34361,8 @@
       <c r="D13" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
     </row>
     <row r="14" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -34487,10 +34487,10 @@
       <c r="D20" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="111" t="s">
+      <c r="E20" s="113" t="s">
         <v>743</v>
       </c>
-      <c r="F20" s="113" t="s">
+      <c r="F20" s="111" t="s">
         <v>744</v>
       </c>
     </row>
@@ -34507,8 +34507,8 @@
       <c r="D21" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="111"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="112"/>
     </row>
     <row r="22" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -35321,10 +35321,10 @@
       <c r="D64" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="113" t="s">
+      <c r="E64" s="111" t="s">
         <v>755</v>
       </c>
-      <c r="F64" s="113" t="s">
+      <c r="F64" s="111" t="s">
         <v>756</v>
       </c>
     </row>
@@ -35341,8 +35341,8 @@
       <c r="D65" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="114"/>
-      <c r="F65" s="114"/>
+      <c r="E65" s="112"/>
+      <c r="F65" s="112"/>
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -35427,10 +35427,10 @@
       <c r="D70" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="111" t="s">
+      <c r="E70" s="113" t="s">
         <v>757</v>
       </c>
-      <c r="F70" s="113" t="s">
+      <c r="F70" s="111" t="s">
         <v>758</v>
       </c>
     </row>
@@ -35447,8 +35447,8 @@
       <c r="D71" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="111"/>
-      <c r="F71" s="114"/>
+      <c r="E71" s="113"/>
+      <c r="F71" s="112"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -35503,10 +35503,10 @@
       <c r="D74" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="113" t="s">
+      <c r="E74" s="111" t="s">
         <v>759</v>
       </c>
-      <c r="F74" s="115" t="s">
+      <c r="F74" s="114" t="s">
         <v>202</v>
       </c>
     </row>
@@ -35523,8 +35523,8 @@
       <c r="D75" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="114"/>
-      <c r="F75" s="114"/>
+      <c r="E75" s="112"/>
+      <c r="F75" s="112"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -36259,10 +36259,10 @@
       <c r="D114" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="113" t="s">
+      <c r="E114" s="111" t="s">
         <v>770</v>
       </c>
-      <c r="F114" s="113" t="s">
+      <c r="F114" s="111" t="s">
         <v>771</v>
       </c>
     </row>
@@ -36279,8 +36279,8 @@
       <c r="D115" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="114"/>
-      <c r="F115" s="114"/>
+      <c r="E115" s="112"/>
+      <c r="F115" s="112"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -37276,22 +37276,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="E64:E65"/>
     <mergeCell ref="E70:E71"/>
@@ -37308,6 +37292,22 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -37371,10 +37371,10 @@
       <c r="D3" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="111" t="s">
         <v>553</v>
       </c>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="111" t="s">
         <v>554</v>
       </c>
     </row>
@@ -37391,8 +37391,8 @@
       <c r="D4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
@@ -37517,10 +37517,10 @@
       <c r="D11" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="111" t="s">
         <v>947</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="111" t="s">
         <v>562</v>
       </c>
     </row>
@@ -37537,8 +37537,8 @@
       <c r="D12" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
     </row>
     <row r="13" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -37553,8 +37553,8 @@
       <c r="D13" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -37569,8 +37569,8 @@
       <c r="D14" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
@@ -37675,10 +37675,10 @@
       <c r="D20" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="113" t="s">
+      <c r="E20" s="111" t="s">
         <v>953</v>
       </c>
-      <c r="F20" s="113" t="s">
+      <c r="F20" s="111" t="s">
         <v>563</v>
       </c>
     </row>
@@ -37695,8 +37695,8 @@
       <c r="D21" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -38619,10 +38619,10 @@
       <c r="D70" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="113" t="s">
+      <c r="E70" s="111" t="s">
         <v>570</v>
       </c>
-      <c r="F70" s="113" t="s">
+      <c r="F70" s="111" t="s">
         <v>571</v>
       </c>
     </row>
@@ -38639,8 +38639,8 @@
       <c r="D71" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="112"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
@@ -38695,10 +38695,10 @@
       <c r="D74" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="108" t="s">
+      <c r="E74" s="106" t="s">
         <v>572</v>
       </c>
-      <c r="F74" s="108" t="s">
+      <c r="F74" s="106" t="s">
         <v>572</v>
       </c>
     </row>
@@ -38715,8 +38715,8 @@
       <c r="D75" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="108"/>
-      <c r="F75" s="108"/>
+      <c r="E75" s="106"/>
+      <c r="F75" s="106"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
@@ -39051,10 +39051,10 @@
       <c r="D93" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="113" t="s">
+      <c r="E93" s="111" t="s">
         <v>580</v>
       </c>
-      <c r="F93" s="113" t="s">
+      <c r="F93" s="111" t="s">
         <v>568</v>
       </c>
     </row>
@@ -39071,8 +39071,8 @@
       <c r="D94" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="114"/>
-      <c r="F94" s="114"/>
+      <c r="E94" s="112"/>
+      <c r="F94" s="112"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
@@ -39447,10 +39447,10 @@
       <c r="D114" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="111" t="s">
+      <c r="E114" s="113" t="s">
         <v>587</v>
       </c>
-      <c r="F114" s="113" t="s">
+      <c r="F114" s="111" t="s">
         <v>588</v>
       </c>
     </row>
@@ -39467,8 +39467,8 @@
       <c r="D115" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="111"/>
-      <c r="F115" s="114"/>
+      <c r="E115" s="113"/>
+      <c r="F115" s="112"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
@@ -40464,6 +40464,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A102:F102"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="E3:E4"/>
@@ -40476,26 +40496,6 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add seabed to raw_data
</commit_message>
<xml_diff>
--- a/rawdata/supplementary_material_V3.xlsx
+++ b/rawdata/supplementary_material_V3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1B0001-6153-4ADF-82F7-12B61A3A7D68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46719F92-4A03-4959-8052-9845F0195DD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="859" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="859" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring system" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10780" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10782" uniqueCount="1044">
   <si>
     <t>Score</t>
   </si>
@@ -4291,6 +4291,9 @@
   </si>
   <si>
     <t>Do you have any paper on the link between unsustainable bottom trawl fisheries and modern slavery and child labor?</t>
+  </si>
+  <si>
+    <t>As targets 1.1 and 1.2 ?</t>
   </si>
 </sst>
 </file>
@@ -4922,12 +4925,6 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4937,11 +4934,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4949,13 +4946,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4967,6 +4970,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4974,15 +4986,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5375,7 +5378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801CB5DA-4450-43AD-9D1A-DDD187F5639A}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
@@ -5429,10 +5432,10 @@
       <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="119" t="s">
         <v>922</v>
       </c>
-      <c r="F3" s="117" t="s">
+      <c r="F3" s="119" t="s">
         <v>601</v>
       </c>
     </row>
@@ -5449,8 +5452,8 @@
       <c r="D4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -5575,10 +5578,10 @@
       <c r="D11" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="117" t="s">
+      <c r="E11" s="119" t="s">
         <v>609</v>
       </c>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="119" t="s">
         <v>610</v>
       </c>
     </row>
@@ -5595,8 +5598,8 @@
       <c r="D12" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -5611,8 +5614,8 @@
       <c r="D13" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -5737,10 +5740,10 @@
       <c r="D20" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="117" t="s">
+      <c r="E20" s="119" t="s">
         <v>613</v>
       </c>
-      <c r="F20" s="117" t="s">
+      <c r="F20" s="119" t="s">
         <v>614</v>
       </c>
     </row>
@@ -5757,8 +5760,8 @@
       <c r="D21" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -6681,10 +6684,10 @@
       <c r="D70" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="117" t="s">
+      <c r="E70" s="119" t="s">
         <v>1040</v>
       </c>
-      <c r="F70" s="117" t="s">
+      <c r="F70" s="119" t="s">
         <v>620</v>
       </c>
     </row>
@@ -6701,8 +6704,8 @@
       <c r="D71" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="117"/>
-      <c r="F71" s="117"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -6987,10 +6990,10 @@
       <c r="D86" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="114" t="s">
+      <c r="E86" s="112" t="s">
         <v>626</v>
       </c>
-      <c r="F86" s="114" t="s">
+      <c r="F86" s="112" t="s">
         <v>627</v>
       </c>
     </row>
@@ -7007,8 +7010,8 @@
       <c r="D87" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="114"/>
-      <c r="F87" s="114"/>
+      <c r="E87" s="112"/>
+      <c r="F87" s="112"/>
     </row>
     <row r="88" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A88" s="22" t="s">
@@ -7023,8 +7026,8 @@
       <c r="D88" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="114"/>
-      <c r="F88" s="114"/>
+      <c r="E88" s="112"/>
+      <c r="F88" s="112"/>
     </row>
     <row r="89" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
@@ -7509,10 +7512,10 @@
       <c r="D114" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="117" t="s">
+      <c r="E114" s="119" t="s">
         <v>630</v>
       </c>
-      <c r="F114" s="117" t="s">
+      <c r="F114" s="119" t="s">
         <v>296</v>
       </c>
     </row>
@@ -7529,8 +7532,8 @@
       <c r="D115" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="117"/>
-      <c r="F115" s="117"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="119"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -8293,10 +8296,10 @@
       <c r="D156" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="117" t="s">
+      <c r="E156" s="119" t="s">
         <v>649</v>
       </c>
-      <c r="F156" s="117" t="s">
+      <c r="F156" s="119" t="s">
         <v>625</v>
       </c>
     </row>
@@ -8313,8 +8316,8 @@
       <c r="D157" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="117"/>
-      <c r="F157" s="117"/>
+      <c r="E157" s="119"/>
+      <c r="F157" s="119"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
@@ -8518,12 +8521,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E156:E157"/>
+    <mergeCell ref="F156:F157"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
     <mergeCell ref="E86:E88"/>
     <mergeCell ref="F86:F88"/>
     <mergeCell ref="A19:F19"/>
@@ -8537,19 +8547,12 @@
     <mergeCell ref="E70:E71"/>
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
-    <mergeCell ref="E156:E157"/>
-    <mergeCell ref="F156:F157"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10001,10 +10004,10 @@
       <c r="D76" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="119" t="s">
+      <c r="E76" s="117" t="s">
         <v>665</v>
       </c>
-      <c r="F76" s="119" t="s">
+      <c r="F76" s="117" t="s">
         <v>666</v>
       </c>
     </row>
@@ -10021,8 +10024,8 @@
       <c r="D77" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="120"/>
-      <c r="F77" s="120"/>
+      <c r="E77" s="118"/>
+      <c r="F77" s="118"/>
     </row>
     <row r="78" spans="1:6" ht="195" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="22" t="s">
@@ -11734,6 +11737,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A10:F10"/>
@@ -11746,14 +11757,6 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="E76:E77"/>
     <mergeCell ref="F76:F77"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11966,10 +11969,10 @@
       <c r="D11" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>691</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="117" t="s">
         <v>933</v>
       </c>
     </row>
@@ -11986,8 +11989,8 @@
       <c r="D12" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
     </row>
     <row r="13" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -12130,10 +12133,10 @@
       <c r="D20" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="117" t="s">
         <v>692</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="117" t="s">
         <v>693</v>
       </c>
     </row>
@@ -12150,8 +12153,8 @@
       <c r="D21" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -13076,10 +13079,10 @@
       <c r="D70" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="117" t="s">
         <v>700</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="117" t="s">
         <v>701</v>
       </c>
     </row>
@@ -13096,8 +13099,8 @@
       <c r="D71" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="118"/>
+      <c r="F71" s="118"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -14302,10 +14305,10 @@
       <c r="D135" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="119" t="s">
+      <c r="E135" s="117" t="s">
         <v>711</v>
       </c>
-      <c r="F135" s="119" t="s">
+      <c r="F135" s="117" t="s">
         <v>702</v>
       </c>
     </row>
@@ -14322,8 +14325,8 @@
       <c r="D136" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E136" s="120"/>
-      <c r="F136" s="120"/>
+      <c r="E136" s="118"/>
+      <c r="F136" s="118"/>
     </row>
     <row r="137" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
@@ -14932,11 +14935,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E135:E136"/>
-    <mergeCell ref="F135:F136"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A33:F33"/>
@@ -14951,13 +14956,11 @@
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14967,8 +14970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC6199F-7BDF-4EB3-87C9-BE284C303509}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162:F162"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14999,14 +15002,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
     </row>
     <row r="3" spans="1:6" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
@@ -15021,10 +15024,10 @@
       <c r="D3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="119" t="s">
+      <c r="E3" s="117" t="s">
         <v>1032</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="117" t="s">
         <v>766</v>
       </c>
     </row>
@@ -15041,8 +15044,8 @@
       <c r="D4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -15113,10 +15116,10 @@
       <c r="D8" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="119" t="s">
+      <c r="E8" s="117" t="s">
         <v>1036</v>
       </c>
-      <c r="F8" s="119" t="s">
+      <c r="F8" s="117" t="s">
         <v>1018</v>
       </c>
     </row>
@@ -15133,8 +15136,8 @@
       <c r="D9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="111" t="s">
@@ -15159,10 +15162,10 @@
       <c r="D11" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="130" t="s">
+      <c r="E11" s="127" t="s">
         <v>1026</v>
       </c>
-      <c r="F11" s="115" t="s">
+      <c r="F11" s="113" t="s">
         <v>1025</v>
       </c>
     </row>
@@ -15179,7 +15182,7 @@
       <c r="D12" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="131"/>
+      <c r="E12" s="129"/>
       <c r="F12" s="124"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
@@ -15195,8 +15198,8 @@
       <c r="D13" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="132"/>
-      <c r="F13" s="116"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="114"/>
     </row>
     <row r="14" spans="1:6" ht="193.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -15321,10 +15324,10 @@
       <c r="D20" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="115" t="s">
+      <c r="E20" s="113" t="s">
         <v>1039</v>
       </c>
-      <c r="F20" s="115" t="s">
+      <c r="F20" s="113" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -15341,8 +15344,8 @@
       <c r="D21" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="116"/>
-      <c r="F21" s="116"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="114"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -15587,7 +15590,7 @@
       <c r="D34" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="127" t="s">
+      <c r="E34" s="130" t="s">
         <v>1042</v>
       </c>
       <c r="F34" s="108" t="s">
@@ -15607,7 +15610,7 @@
       <c r="D35" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="129"/>
+      <c r="E35" s="132"/>
       <c r="F35" s="108" t="s">
         <v>29</v>
       </c>
@@ -15625,7 +15628,7 @@
       <c r="D36" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="129"/>
+      <c r="E36" s="132"/>
       <c r="F36" s="108" t="s">
         <v>29</v>
       </c>
@@ -15643,7 +15646,7 @@
       <c r="D37" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="128"/>
+      <c r="E37" s="131"/>
       <c r="F37" s="108" t="s">
         <v>29</v>
       </c>
@@ -16245,14 +16248,18 @@
       <c r="B70" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="C70" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E70" s="44"/>
-      <c r="F70" s="106"/>
+      <c r="C70" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="117" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F70" s="117" t="s">
+        <v>1043</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A71" s="22" t="s">
@@ -16261,14 +16268,14 @@
       <c r="B71" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="C71" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E71" s="44"/>
-      <c r="F71" s="106"/>
+      <c r="C71" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="118"/>
+      <c r="F71" s="118"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -17035,10 +17042,10 @@
       <c r="D114" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="117" t="s">
+      <c r="E114" s="119" t="s">
         <v>1041</v>
       </c>
-      <c r="F114" s="117" t="s">
+      <c r="F114" s="119" t="s">
         <v>296</v>
       </c>
     </row>
@@ -17055,8 +17062,8 @@
       <c r="D115" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="117"/>
-      <c r="F115" s="117"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="119"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -17259,10 +17266,10 @@
       <c r="D126" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="115" t="s">
+      <c r="E126" s="113" t="s">
         <v>1015</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="113" t="s">
         <v>1016</v>
       </c>
     </row>
@@ -17295,8 +17302,8 @@
       <c r="D128" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E128" s="116"/>
-      <c r="F128" s="116"/>
+      <c r="E128" s="114"/>
+      <c r="F128" s="114"/>
     </row>
     <row r="129" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
@@ -17361,10 +17368,10 @@
       <c r="D132" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="130" t="s">
+      <c r="E132" s="127" t="s">
         <v>1022</v>
       </c>
-      <c r="F132" s="130" t="s">
+      <c r="F132" s="127" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -17381,8 +17388,8 @@
       <c r="D133" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="132"/>
-      <c r="F133" s="132"/>
+      <c r="E133" s="128"/>
+      <c r="F133" s="128"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -17803,7 +17810,7 @@
       <c r="D156" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="127" t="s">
+      <c r="E156" s="130" t="s">
         <v>1042</v>
       </c>
       <c r="F156" s="106"/>
@@ -17821,7 +17828,7 @@
       <c r="D157" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="128"/>
+      <c r="E157" s="131"/>
       <c r="F157" s="106"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -17989,23 +17996,9 @@
       <c r="F167" s="106"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E126:E128"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F126:F128"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+  <mergeCells count="34">
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
     <mergeCell ref="E156:E157"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="F20:F21"/>
@@ -18022,6 +18015,22 @@
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E126:E128"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F126:F128"/>
+    <mergeCell ref="F132:F133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18065,14 +18074,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
@@ -20425,10 +20434,10 @@
       <c r="D126" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="114" t="s">
+      <c r="E126" s="112" t="s">
         <v>452</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="113" t="s">
         <v>453</v>
       </c>
     </row>
@@ -20445,8 +20454,8 @@
       <c r="D127" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="114"/>
-      <c r="F127" s="116"/>
+      <c r="E127" s="112"/>
+      <c r="F127" s="114"/>
     </row>
     <row r="128" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -21220,6 +21229,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="A69:F69"/>
@@ -21232,12 +21247,6 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21301,10 +21310,10 @@
       <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="114" t="s">
+      <c r="E3" s="112" t="s">
         <v>919</v>
       </c>
-      <c r="F3" s="114" t="s">
+      <c r="F3" s="112" t="s">
         <v>920</v>
       </c>
     </row>
@@ -21321,8 +21330,8 @@
       <c r="D4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
     </row>
     <row r="5" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -21447,10 +21456,10 @@
       <c r="D11" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="119" t="s">
         <v>928</v>
       </c>
     </row>
@@ -21467,8 +21476,8 @@
       <c r="D12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
     </row>
     <row r="13" spans="1:6" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -21483,8 +21492,8 @@
       <c r="D13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
     </row>
     <row r="14" spans="1:6" ht="228.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -22551,10 +22560,10 @@
       <c r="D70" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="114" t="s">
+      <c r="E70" s="112" t="s">
         <v>190</v>
       </c>
-      <c r="F70" s="114" t="s">
+      <c r="F70" s="112" t="s">
         <v>191</v>
       </c>
     </row>
@@ -22571,8 +22580,8 @@
       <c r="D71" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="114"/>
-      <c r="F71" s="114"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="112"/>
     </row>
     <row r="72" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -23387,10 +23396,10 @@
       <c r="D114" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="117" t="s">
+      <c r="E114" s="119" t="s">
         <v>295</v>
       </c>
-      <c r="F114" s="117" t="s">
+      <c r="F114" s="119" t="s">
         <v>296</v>
       </c>
     </row>
@@ -23407,8 +23416,8 @@
       <c r="D115" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="117"/>
-      <c r="F115" s="117"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="119"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -23613,10 +23622,10 @@
       <c r="D126" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="117" t="s">
+      <c r="E126" s="119" t="s">
         <v>322</v>
       </c>
-      <c r="F126" s="117" t="s">
+      <c r="F126" s="119" t="s">
         <v>323</v>
       </c>
     </row>
@@ -23633,8 +23642,8 @@
       <c r="D127" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="117"/>
-      <c r="F127" s="117"/>
+      <c r="E127" s="119"/>
+      <c r="F127" s="119"/>
     </row>
     <row r="128" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -23719,10 +23728,10 @@
       <c r="D132" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="117" t="s">
+      <c r="E132" s="119" t="s">
         <v>335</v>
       </c>
-      <c r="F132" s="117" t="s">
+      <c r="F132" s="119" t="s">
         <v>336</v>
       </c>
     </row>
@@ -23739,8 +23748,8 @@
       <c r="D133" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="117"/>
-      <c r="F133" s="117"/>
+      <c r="E133" s="119"/>
+      <c r="F133" s="119"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -24105,10 +24114,10 @@
       <c r="D152" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="118" t="s">
+      <c r="E152" s="121" t="s">
         <v>387</v>
       </c>
-      <c r="F152" s="118" t="s">
+      <c r="F152" s="121" t="s">
         <v>388</v>
       </c>
     </row>
@@ -24125,8 +24134,8 @@
       <c r="D153" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="118"/>
-      <c r="F153" s="118"/>
+      <c r="E153" s="121"/>
+      <c r="F153" s="121"/>
     </row>
     <row r="154" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="22" t="s">
@@ -24171,10 +24180,10 @@
       <c r="D156" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="119" t="s">
+      <c r="E156" s="117" t="s">
         <v>397</v>
       </c>
-      <c r="F156" s="119" t="s">
+      <c r="F156" s="117" t="s">
         <v>398</v>
       </c>
     </row>
@@ -24191,8 +24200,8 @@
       <c r="D157" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="120"/>
-      <c r="F157" s="120"/>
+      <c r="E157" s="118"/>
+      <c r="F157" s="118"/>
     </row>
     <row r="158" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
@@ -24396,6 +24405,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F156:F157"/>
     <mergeCell ref="E156:E157"/>
@@ -24412,22 +24437,6 @@
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="A125:F125"/>
     <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -24499,10 +24508,10 @@
       <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="119" t="s">
         <v>921</v>
       </c>
-      <c r="F3" s="117" t="s">
+      <c r="F3" s="119" t="s">
         <v>465</v>
       </c>
     </row>
@@ -24519,8 +24528,8 @@
       <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -24645,10 +24654,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="117" t="s">
+      <c r="E11" s="119" t="s">
         <v>469</v>
       </c>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="119" t="s">
         <v>470</v>
       </c>
     </row>
@@ -24665,8 +24674,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -24681,8 +24690,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -25646,10 +25655,10 @@
       <c r="D64" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="117" t="s">
+      <c r="E64" s="119" t="s">
         <v>486</v>
       </c>
-      <c r="F64" s="117" t="s">
+      <c r="F64" s="119" t="s">
         <v>487</v>
       </c>
     </row>
@@ -25666,8 +25675,8 @@
       <c r="D65" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="117"/>
-      <c r="F65" s="117"/>
+      <c r="E65" s="119"/>
+      <c r="F65" s="119"/>
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="22" t="s">
@@ -25752,10 +25761,10 @@
       <c r="D70" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E70" s="117" t="s">
+      <c r="E70" s="119" t="s">
         <v>947</v>
       </c>
-      <c r="F70" s="117" t="s">
+      <c r="F70" s="119" t="s">
         <v>948</v>
       </c>
       <c r="G70" s="60"/>
@@ -25773,8 +25782,8 @@
       <c r="D71" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="117"/>
-      <c r="F71" s="117"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
       <c r="G71" s="60"/>
     </row>
     <row r="72" spans="1:7" ht="78" x14ac:dyDescent="0.3">
@@ -26592,10 +26601,10 @@
       <c r="D114" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="122" t="s">
+      <c r="E114" s="123" t="s">
         <v>491</v>
       </c>
-      <c r="F114" s="114" t="s">
+      <c r="F114" s="112" t="s">
         <v>492</v>
       </c>
     </row>
@@ -26612,8 +26621,8 @@
       <c r="D115" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="122"/>
-      <c r="F115" s="114"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="112"/>
     </row>
     <row r="116" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -26818,10 +26827,10 @@
       <c r="D126" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="114" t="s">
+      <c r="E126" s="112" t="s">
         <v>495</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="113" t="s">
         <v>496</v>
       </c>
     </row>
@@ -26838,8 +26847,8 @@
       <c r="D127" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="114"/>
-      <c r="F127" s="116"/>
+      <c r="E127" s="112"/>
+      <c r="F127" s="114"/>
     </row>
     <row r="128" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -26923,10 +26932,10 @@
       <c r="D132" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="114" t="s">
+      <c r="E132" s="112" t="s">
         <v>497</v>
       </c>
-      <c r="F132" s="114" t="s">
+      <c r="F132" s="112" t="s">
         <v>498</v>
       </c>
     </row>
@@ -26943,8 +26952,8 @@
       <c r="D133" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="114"/>
-      <c r="F133" s="114"/>
+      <c r="E133" s="112"/>
+      <c r="F133" s="112"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -26959,8 +26968,8 @@
       <c r="D134" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="114"/>
-      <c r="F134" s="114"/>
+      <c r="E134" s="112"/>
+      <c r="F134" s="112"/>
     </row>
     <row r="135" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
@@ -27128,7 +27137,7 @@
       <c r="E143" s="27" t="s">
         <v>499</v>
       </c>
-      <c r="F143" s="117" t="s">
+      <c r="F143" s="119" t="s">
         <v>366</v>
       </c>
     </row>
@@ -27148,7 +27157,7 @@
       <c r="E144" s="27" t="s">
         <v>500</v>
       </c>
-      <c r="F144" s="117"/>
+      <c r="F144" s="119"/>
     </row>
     <row r="145" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A145" s="22" t="s">
@@ -27263,10 +27272,10 @@
       <c r="D150" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E150" s="115" t="s">
+      <c r="E150" s="113" t="s">
         <v>506</v>
       </c>
-      <c r="F150" s="115" t="s">
+      <c r="F150" s="113" t="s">
         <v>507</v>
       </c>
       <c r="G150" s="64"/>
@@ -27284,8 +27293,8 @@
       <c r="D151" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E151" s="116"/>
-      <c r="F151" s="116"/>
+      <c r="E151" s="114"/>
+      <c r="F151" s="114"/>
       <c r="G151" s="60"/>
     </row>
     <row r="152" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -27301,10 +27310,10 @@
       <c r="D152" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E152" s="123" t="s">
+      <c r="E152" s="122" t="s">
         <v>508</v>
       </c>
-      <c r="F152" s="123" t="s">
+      <c r="F152" s="122" t="s">
         <v>484</v>
       </c>
     </row>
@@ -27321,8 +27330,8 @@
       <c r="D153" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E153" s="123"/>
-      <c r="F153" s="123"/>
+      <c r="E153" s="122"/>
+      <c r="F153" s="122"/>
     </row>
     <row r="154" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A154" s="22" t="s">
@@ -27596,22 +27605,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E134"/>
-    <mergeCell ref="F132:F134"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -27625,12 +27624,22 @@
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27694,10 +27703,10 @@
       <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="119" t="s">
         <v>510</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="117" t="s">
         <v>511</v>
       </c>
     </row>
@@ -27714,8 +27723,8 @@
       <c r="D4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="118"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -27840,10 +27849,10 @@
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>515</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="117" t="s">
         <v>516</v>
       </c>
     </row>
@@ -27860,8 +27869,8 @@
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
     </row>
     <row r="13" spans="1:6" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -27876,8 +27885,8 @@
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
     </row>
     <row r="14" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -28942,10 +28951,10 @@
       <c r="D70" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="117" t="s">
         <v>526</v>
       </c>
-      <c r="F70" s="115" t="s">
+      <c r="F70" s="113" t="s">
         <v>527</v>
       </c>
     </row>
@@ -28962,7 +28971,7 @@
       <c r="D71" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="120"/>
+      <c r="E71" s="118"/>
       <c r="F71" s="124"/>
     </row>
     <row r="72" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -30004,10 +30013,10 @@
       <c r="D126" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E126" s="114" t="s">
+      <c r="E126" s="112" t="s">
         <v>534</v>
       </c>
-      <c r="F126" s="115" t="s">
+      <c r="F126" s="113" t="s">
         <v>535</v>
       </c>
     </row>
@@ -30024,8 +30033,8 @@
       <c r="D127" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="114"/>
-      <c r="F127" s="116"/>
+      <c r="E127" s="112"/>
+      <c r="F127" s="114"/>
     </row>
     <row r="128" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
@@ -30108,10 +30117,10 @@
       <c r="D132" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="114" t="s">
+      <c r="E132" s="112" t="s">
         <v>536</v>
       </c>
-      <c r="F132" s="115" t="s">
+      <c r="F132" s="113" t="s">
         <v>537</v>
       </c>
     </row>
@@ -30128,8 +30137,8 @@
       <c r="D133" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="114"/>
-      <c r="F133" s="116"/>
+      <c r="E133" s="112"/>
+      <c r="F133" s="114"/>
     </row>
     <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
@@ -30624,10 +30633,10 @@
       <c r="D159" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="114" t="s">
+      <c r="E159" s="112" t="s">
         <v>547</v>
       </c>
-      <c r="F159" s="115" t="s">
+      <c r="F159" s="113" t="s">
         <v>982</v>
       </c>
     </row>
@@ -30644,8 +30653,8 @@
       <c r="D160" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="114"/>
-      <c r="F160" s="116"/>
+      <c r="E160" s="112"/>
+      <c r="F160" s="114"/>
     </row>
     <row r="161" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A161" s="22" t="s">
@@ -30789,12 +30798,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
     <mergeCell ref="A113:F113"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A33:F33"/>
@@ -30807,16 +30820,12 @@
     <mergeCell ref="A82:F82"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31029,10 +31038,10 @@
       <c r="D11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="117" t="s">
+      <c r="E11" s="119" t="s">
         <v>906</v>
       </c>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="119" t="s">
         <v>1013</v>
       </c>
     </row>
@@ -31049,8 +31058,8 @@
       <c r="D12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="150.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -31195,10 +31204,10 @@
       <c r="D20" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="114" t="s">
+      <c r="E20" s="112" t="s">
         <v>840</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="112" t="s">
         <v>841</v>
       </c>
     </row>
@@ -31215,8 +31224,8 @@
       <c r="D21" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
     </row>
     <row r="22" spans="1:6" ht="200.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -31879,10 +31888,10 @@
       <c r="D56" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="117" t="s">
+      <c r="E56" s="119" t="s">
         <v>847</v>
       </c>
-      <c r="F56" s="117" t="s">
+      <c r="F56" s="119" t="s">
         <v>848</v>
       </c>
     </row>
@@ -31899,8 +31908,8 @@
       <c r="D57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="117"/>
-      <c r="F57" s="117"/>
+      <c r="E57" s="119"/>
+      <c r="F57" s="119"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
@@ -32135,10 +32144,10 @@
       <c r="D70" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="117" t="s">
+      <c r="E70" s="119" t="s">
         <v>910</v>
       </c>
-      <c r="F70" s="117" t="s">
+      <c r="F70" s="119" t="s">
         <v>989</v>
       </c>
     </row>
@@ -32155,8 +32164,8 @@
       <c r="D71" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="117"/>
-      <c r="F71" s="117"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -32211,10 +32220,10 @@
       <c r="D74" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="114" t="s">
+      <c r="E74" s="112" t="s">
         <v>970</v>
       </c>
-      <c r="F74" s="114" t="s">
+      <c r="F74" s="112" t="s">
         <v>851</v>
       </c>
     </row>
@@ -32231,8 +32240,8 @@
       <c r="D75" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="114"/>
-      <c r="F75" s="114"/>
+      <c r="E75" s="112"/>
+      <c r="F75" s="112"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -32567,10 +32576,10 @@
       <c r="D93" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="115" t="s">
+      <c r="E93" s="113" t="s">
         <v>855</v>
       </c>
-      <c r="F93" s="115" t="s">
+      <c r="F93" s="113" t="s">
         <v>856</v>
       </c>
     </row>
@@ -32587,8 +32596,8 @@
       <c r="D94" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="116"/>
-      <c r="F94" s="116"/>
+      <c r="E94" s="114"/>
+      <c r="F94" s="114"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="22" t="s">
@@ -32963,10 +32972,10 @@
       <c r="D114" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="114" t="s">
+      <c r="E114" s="112" t="s">
         <v>864</v>
       </c>
-      <c r="F114" s="114" t="s">
+      <c r="F114" s="112" t="s">
         <v>865</v>
       </c>
     </row>
@@ -32983,8 +32992,8 @@
       <c r="D115" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="114"/>
-      <c r="F115" s="114"/>
+      <c r="E115" s="112"/>
+      <c r="F115" s="112"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -33528,7 +33537,7 @@
       <c r="E144" s="89" t="s">
         <v>878</v>
       </c>
-      <c r="F144" s="117" t="s">
+      <c r="F144" s="119" t="s">
         <v>36</v>
       </c>
     </row>
@@ -33548,7 +33557,7 @@
       <c r="E145" s="89" t="s">
         <v>879</v>
       </c>
-      <c r="F145" s="117"/>
+      <c r="F145" s="119"/>
     </row>
     <row r="146" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A146" s="22" t="s">
@@ -33976,15 +33985,19 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="F114:F115"/>
     <mergeCell ref="A69:F69"/>
@@ -33998,19 +34011,15 @@
     <mergeCell ref="F93:F94"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="F144:F145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34225,10 +34234,10 @@
       <c r="D11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>786</v>
       </c>
-      <c r="F11" s="117" t="s">
+      <c r="F11" s="119" t="s">
         <v>787</v>
       </c>
     </row>
@@ -34245,8 +34254,8 @@
       <c r="D12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="120"/>
-      <c r="F12" s="117"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -34391,10 +34400,10 @@
       <c r="D20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="114" t="s">
+      <c r="E20" s="112" t="s">
         <v>899</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="112" t="s">
         <v>935</v>
       </c>
     </row>
@@ -34411,8 +34420,8 @@
       <c r="D21" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
     </row>
     <row r="22" spans="1:6" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -35075,10 +35084,10 @@
       <c r="D56" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="119" t="s">
+      <c r="E56" s="117" t="s">
         <v>897</v>
       </c>
-      <c r="F56" s="119" t="s">
+      <c r="F56" s="117" t="s">
         <v>898</v>
       </c>
     </row>
@@ -35095,8 +35104,8 @@
       <c r="D57" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="120"/>
-      <c r="F57" s="120"/>
+      <c r="E57" s="118"/>
+      <c r="F57" s="118"/>
     </row>
     <row r="58" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
@@ -35331,10 +35340,10 @@
       <c r="D70" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="117" t="s">
         <v>799</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="117" t="s">
         <v>800</v>
       </c>
     </row>
@@ -35351,8 +35360,8 @@
       <c r="D71" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="118"/>
+      <c r="F71" s="118"/>
     </row>
     <row r="72" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -35407,10 +35416,10 @@
       <c r="D74" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="115" t="s">
+      <c r="E74" s="113" t="s">
         <v>802</v>
       </c>
-      <c r="F74" s="115" t="s">
+      <c r="F74" s="113" t="s">
         <v>801</v>
       </c>
     </row>
@@ -35427,8 +35436,8 @@
       <c r="D75" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="116"/>
-      <c r="F75" s="116"/>
+      <c r="E75" s="114"/>
+      <c r="F75" s="114"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -36163,10 +36172,10 @@
       <c r="D114" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="114" t="s">
+      <c r="E114" s="112" t="s">
         <v>811</v>
       </c>
-      <c r="F114" s="115" t="s">
+      <c r="F114" s="113" t="s">
         <v>812</v>
       </c>
     </row>
@@ -36183,8 +36192,8 @@
       <c r="D115" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="114"/>
-      <c r="F115" s="116"/>
+      <c r="E115" s="112"/>
+      <c r="F115" s="114"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -37178,6 +37187,28 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="E74:E75"/>
     <mergeCell ref="F152:F153"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="F114:F115"/>
@@ -37188,28 +37219,6 @@
     <mergeCell ref="E114:E115"/>
     <mergeCell ref="E126:E127"/>
     <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -37273,10 +37282,10 @@
       <c r="D3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="119" t="s">
         <v>720</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="117" t="s">
         <v>721</v>
       </c>
     </row>
@@ -37293,8 +37302,8 @@
       <c r="D4" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="118"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -37419,10 +37428,10 @@
       <c r="D11" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>929</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="117" t="s">
         <v>726</v>
       </c>
     </row>
@@ -37439,8 +37448,8 @@
       <c r="D12" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -37455,8 +37464,8 @@
       <c r="D13" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
     </row>
     <row r="14" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -37581,10 +37590,10 @@
       <c r="D20" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="117" t="s">
+      <c r="E20" s="119" t="s">
         <v>729</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="117" t="s">
         <v>730</v>
       </c>
     </row>
@@ -37601,8 +37610,8 @@
       <c r="D21" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="117"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="118"/>
     </row>
     <row r="22" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -38415,10 +38424,10 @@
       <c r="D64" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="119" t="s">
+      <c r="E64" s="117" t="s">
         <v>740</v>
       </c>
-      <c r="F64" s="119" t="s">
+      <c r="F64" s="117" t="s">
         <v>741</v>
       </c>
     </row>
@@ -38435,8 +38444,8 @@
       <c r="D65" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="120"/>
-      <c r="F65" s="120"/>
+      <c r="E65" s="118"/>
+      <c r="F65" s="118"/>
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="22" t="s">
@@ -38521,10 +38530,10 @@
       <c r="D70" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="117" t="s">
+      <c r="E70" s="119" t="s">
         <v>742</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="117" t="s">
         <v>743</v>
       </c>
     </row>
@@ -38541,8 +38550,8 @@
       <c r="D71" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="117"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="118"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -38597,10 +38606,10 @@
       <c r="D74" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="119" t="s">
+      <c r="E74" s="117" t="s">
         <v>744</v>
       </c>
-      <c r="F74" s="121" t="s">
+      <c r="F74" s="120" t="s">
         <v>200</v>
       </c>
     </row>
@@ -38617,8 +38626,8 @@
       <c r="D75" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="120"/>
-      <c r="F75" s="120"/>
+      <c r="E75" s="118"/>
+      <c r="F75" s="118"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -39353,10 +39362,10 @@
       <c r="D114" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="119" t="s">
+      <c r="E114" s="117" t="s">
         <v>755</v>
       </c>
-      <c r="F114" s="119" t="s">
+      <c r="F114" s="117" t="s">
         <v>756</v>
       </c>
     </row>
@@ -39373,8 +39382,8 @@
       <c r="D115" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="120"/>
-      <c r="F115" s="120"/>
+      <c r="E115" s="118"/>
+      <c r="F115" s="118"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -40370,22 +40379,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F20:F21"/>
     <mergeCell ref="A155:F155"/>
     <mergeCell ref="E64:E65"/>
     <mergeCell ref="E70:E71"/>
@@ -40402,6 +40395,22 @@
     <mergeCell ref="F126:F127"/>
     <mergeCell ref="A131:F131"/>
     <mergeCell ref="A142:F142"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40465,10 +40474,10 @@
       <c r="D3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="119" t="s">
+      <c r="E3" s="117" t="s">
         <v>550</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="117" t="s">
         <v>551</v>
       </c>
     </row>
@@ -40485,8 +40494,8 @@
       <c r="D4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
     </row>
     <row r="5" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -40611,10 +40620,10 @@
       <c r="D11" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>930</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="117" t="s">
         <v>559</v>
       </c>
     </row>
@@ -40631,8 +40640,8 @@
       <c r="D12" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
     </row>
     <row r="13" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -40647,8 +40656,8 @@
       <c r="D13" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -40663,8 +40672,8 @@
       <c r="D14" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
     </row>
     <row r="15" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
@@ -40769,10 +40778,10 @@
       <c r="D20" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="117" t="s">
         <v>936</v>
       </c>
-      <c r="F20" s="119" t="s">
+      <c r="F20" s="117" t="s">
         <v>560</v>
       </c>
     </row>
@@ -40789,8 +40798,8 @@
       <c r="D21" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
     </row>
     <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
@@ -41713,10 +41722,10 @@
       <c r="D70" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="119" t="s">
+      <c r="E70" s="117" t="s">
         <v>567</v>
       </c>
-      <c r="F70" s="119" t="s">
+      <c r="F70" s="117" t="s">
         <v>568</v>
       </c>
     </row>
@@ -41733,8 +41742,8 @@
       <c r="D71" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="120"/>
-      <c r="F71" s="120"/>
+      <c r="E71" s="118"/>
+      <c r="F71" s="118"/>
     </row>
     <row r="72" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
@@ -41789,10 +41798,10 @@
       <c r="D74" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="114" t="s">
+      <c r="E74" s="112" t="s">
         <v>569</v>
       </c>
-      <c r="F74" s="114" t="s">
+      <c r="F74" s="112" t="s">
         <v>569</v>
       </c>
     </row>
@@ -41809,8 +41818,8 @@
       <c r="D75" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="114"/>
-      <c r="F75" s="114"/>
+      <c r="E75" s="112"/>
+      <c r="F75" s="112"/>
     </row>
     <row r="76" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
@@ -42145,10 +42154,10 @@
       <c r="D93" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="119" t="s">
+      <c r="E93" s="117" t="s">
         <v>577</v>
       </c>
-      <c r="F93" s="119" t="s">
+      <c r="F93" s="117" t="s">
         <v>565</v>
       </c>
     </row>
@@ -42165,8 +42174,8 @@
       <c r="D94" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="120"/>
-      <c r="F94" s="120"/>
+      <c r="E94" s="118"/>
+      <c r="F94" s="118"/>
     </row>
     <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="22" t="s">
@@ -42541,10 +42550,10 @@
       <c r="D114" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="117" t="s">
+      <c r="E114" s="119" t="s">
         <v>584</v>
       </c>
-      <c r="F114" s="119" t="s">
+      <c r="F114" s="117" t="s">
         <v>585</v>
       </c>
     </row>
@@ -42561,8 +42570,8 @@
       <c r="D115" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="117"/>
-      <c r="F115" s="120"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="118"/>
     </row>
     <row r="116" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
@@ -43558,6 +43567,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A142:F142"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="A125:F125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="A131:F131"/>
+    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A102:F102"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="E3:E4"/>
@@ -43570,26 +43599,6 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A113:F113"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="A142:F142"/>
-    <mergeCell ref="A155:F155"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="A125:F125"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="A131:F131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>